<commit_message>
Main PCB update: - edge cuts: yet another update hopefully getting the perfect fit this time - hdmi connector position moved 0.5mm to the left - optimize mask for D21, D22, X3
</commit_message>
<xml_diff>
--- a/doc/n64adv2_BOM.xlsx
+++ b/doc/n64adv2_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\GitHub\n64rgb_project\n64adv2_pcb\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBCF5DD-8951-4683-B7CF-CC9124203003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C53A2C7-8B92-4D01-BECB-37B79552F51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1577,7 +1577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3865,7 +3865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395CB06B-4E35-4D83-939D-902BBC6C7ADF}">
   <dimension ref="A2:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
update part numbers for Y41,, RN11-14
</commit_message>
<xml_diff>
--- a/doc/n64adv2_BOM.xlsx
+++ b/doc/n64adv2_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\GitHub\n64rgb_project\n64adv2_pcb\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0565ED-935C-4E27-AFE0-44B386A2D0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DEA19C-1924-47E3-82FC-0DB5DDB76897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9645" yWindow="2820" windowWidth="25005" windowHeight="13980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -164,9 +164,6 @@
     <t>3,0mm x 4,5mm pad</t>
   </si>
   <si>
-    <t xml:space="preserve">BK32164M121-T </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ferrite Beads MULTILYR CHP </t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>U12</t>
   </si>
   <si>
-    <t>7A-27.000MAAJ-T</t>
-  </si>
-  <si>
     <t>27MHz crystal</t>
   </si>
   <si>
@@ -732,6 +726,12 @@
   </si>
   <si>
     <t>Set both banks to 2.5V in current setup! (shorted since N64Adv2_20220729 anyway)</t>
+  </si>
+  <si>
+    <t>445I23D27M00000</t>
+  </si>
+  <si>
+    <t>BLA31AG121SN4D</t>
   </si>
 </sst>
 </file>
@@ -1230,28 +1230,22 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" quotePrefix="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1577,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1590,118 +1584,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="9"/>
       <c r="C1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <f>$C$1*C4</f>
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F4"/>
       <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="H4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5"/>
       <c r="E5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="F5"/>
       <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="H5" t="s">
+        <v>217</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <f t="shared" ref="D6:D61" si="0">$C$1*C6</f>
         <v>3</v>
       </c>
       <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
         <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1711,23 +1705,23 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1736,21 +1730,21 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>86</v>
+      <c r="B8" t="s">
+        <v>85</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <f>$C$1*C8</f>
         <v>3</v>
       </c>
       <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" t="s">
         <v>84</v>
-      </c>
-      <c r="G8" t="s">
-        <v>85</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1759,18 +1753,18 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>77</v>
+      <c r="B9" t="s">
+        <v>76</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
@@ -1782,32 +1776,31 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="5"/>
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
       <c r="H10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
@@ -1819,64 +1812,61 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D12" s="5"/>
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
       <c r="H12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="D14" s="5"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
         <v>87</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
@@ -1886,37 +1876,36 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>127</v>
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>125</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G16" t="s">
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="5"/>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
       <c r="E17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G17" t="s">
         <v>19</v>
@@ -1926,20 +1915,20 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
         <v>19</v>
@@ -1947,55 +1936,49 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="5"/>
-    </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>229</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="5"/>
+        <v>91</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -2003,7 +1986,7 @@
       <c r="C23">
         <v>14</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
@@ -2013,21 +1996,18 @@
       <c r="G23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2045,15 +2025,15 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C26">
         <v>9</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -2071,15 +2051,15 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B27" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C27">
         <v>8</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
@@ -2097,15 +2077,15 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C28">
         <v>49</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28">
         <f t="shared" si="0"/>
         <v>147</v>
       </c>
@@ -2123,15 +2103,15 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2148,21 +2128,20 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D30" s="5"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>116</v>
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>114</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2170,7 +2149,7 @@
         <v>31</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" t="s">
         <v>27</v>
@@ -2180,15 +2159,15 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>115</v>
+        <v>92</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2206,15 +2185,15 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>117</v>
+        <v>146</v>
+      </c>
+      <c r="B33" t="s">
+        <v>115</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2222,36 +2201,36 @@
         <v>31</v>
       </c>
       <c r="F33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
         <v>27</v>
       </c>
       <c r="H33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>118</v>
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>116</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E34" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>57</v>
+      <c r="F34" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="G34" t="s">
         <v>27</v>
@@ -2259,42 +2238,42 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>149</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>119</v>
+        <v>147</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E35" t="s">
         <v>31</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>98</v>
+      <c r="F35" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G35" t="s">
         <v>27</v>
       </c>
       <c r="H35" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>150</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>120</v>
+        <v>148</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2302,7 +2281,7 @@
         <v>31</v>
       </c>
       <c r="F36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G36" t="s">
         <v>27</v>
@@ -2314,489 +2293,457 @@
       <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>121</v>
+      <c r="B37" t="s">
+        <v>119</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E37" t="s">
         <v>31</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>58</v>
+      <c r="F37" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="G37" t="s">
         <v>27</v>
       </c>
-      <c r="H37" s="5"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>197</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E38" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>51</v>
+      <c r="F38" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G38" t="s">
         <v>27</v>
       </c>
-      <c r="H38" s="5"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>151</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="B39" t="s">
+        <v>150</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E39" t="s">
         <v>31</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>153</v>
+      <c r="F39" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="G39" t="s">
         <v>27</v>
       </c>
-      <c r="H39" s="5"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D40" s="5"/>
-      <c r="H40" s="5"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>230</v>
       </c>
       <c r="C41">
         <v>4</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="5"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>101</v>
-      </c>
-      <c r="B42" s="5" t="s">
         <v>99</v>
+      </c>
+      <c r="B42" t="s">
+        <v>97</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G42" s="5" t="s">
+      <c r="F42" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G42" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>154</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>102</v>
+        <v>152</v>
+      </c>
+      <c r="B43" t="s">
+        <v>100</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" t="s">
         <v>34</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G43" s="5" t="s">
+      <c r="F43" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43" t="s">
         <v>15</v>
       </c>
-      <c r="H43" s="5"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D44" s="5"/>
-      <c r="H44" s="5"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="5">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F45" s="6"/>
-      <c r="G45" s="5" t="s">
+      <c r="E45" t="s">
+        <v>63</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" t="s">
         <v>27</v>
       </c>
-      <c r="H45" s="10"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="I45" s="4"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
         <v>104</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" s="5">
+      <c r="C46">
         <v>1</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F46" s="6"/>
-      <c r="G46" s="5" t="s">
+      <c r="E46" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" t="s">
         <v>16</v>
       </c>
-      <c r="H46" s="10"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="8"/>
-    </row>
-    <row r="47" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="I46" s="4"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
         <v>105</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C47" s="5">
+      <c r="C47">
         <v>1</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E47" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="5" t="s">
+      <c r="E47" t="s">
+        <v>107</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="10"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="5" t="s">
+      <c r="I47" s="4"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" t="s">
+        <v>196</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" t="s">
         <v>16</v>
       </c>
-      <c r="H48" s="10"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>60</v>
+      <c r="I48" s="4"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="5">
+        <v>61</v>
+      </c>
+      <c r="C49">
         <v>2</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" t="s">
+        <v>62</v>
+      </c>
+      <c r="I49" s="4"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" t="s">
+        <v>62</v>
+      </c>
+      <c r="H50" t="s">
+        <v>71</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H49" s="10"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="8"/>
-    </row>
-    <row r="50" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>143</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="I50" s="7"/>
-      <c r="J50" s="8"/>
-    </row>
-    <row r="51" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="B51" t="s">
-        <v>144</v>
-      </c>
-      <c r="C51" s="5">
+        <v>142</v>
+      </c>
+      <c r="C51">
         <v>1</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D51">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="5" t="s">
+      <c r="E51" t="s">
+        <v>144</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" t="s">
+        <v>143</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="4"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
         <v>145</v>
       </c>
-      <c r="H51" s="10"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="8"/>
-    </row>
-    <row r="52" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H52" s="10"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="8"/>
-    </row>
-    <row r="53" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C53" s="5">
+      <c r="C53">
         <v>2</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D53">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E53" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H53" s="10"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="8"/>
-    </row>
-    <row r="54" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H54" s="10"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="8"/>
-    </row>
-    <row r="55" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C55" s="5">
+      <c r="E53" t="s">
+        <v>109</v>
+      </c>
+      <c r="G53" t="s">
+        <v>110</v>
+      </c>
+      <c r="I53" s="4"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="4"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55">
         <v>1</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="F55" s="6"/>
-      <c r="H55" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="I55" s="7"/>
-      <c r="J55" s="8"/>
-    </row>
-    <row r="56" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56"/>
-      <c r="F56" s="6"/>
-      <c r="H56" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I56" s="7"/>
-      <c r="J56" s="8"/>
-    </row>
-    <row r="57" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="9"/>
-      <c r="F57" s="6"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="8"/>
-    </row>
-    <row r="58" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C58" s="5">
+      <c r="E55" t="s">
+        <v>188</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="H55" t="s">
+        <v>189</v>
+      </c>
+      <c r="I55" s="4"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F56" s="2"/>
+      <c r="H56" t="s">
+        <v>129</v>
+      </c>
+      <c r="I56" s="4"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="6"/>
+      <c r="F57" s="2"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C58">
         <v>1</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58">
         <f>$C$1*C58</f>
         <v>3</v>
       </c>
-      <c r="F58" s="6"/>
-      <c r="H58" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="I58" s="7"/>
-      <c r="J58" s="8"/>
-    </row>
-    <row r="59" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="2"/>
+      <c r="H58" t="s">
+        <v>198</v>
+      </c>
+      <c r="I58" s="4"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>35</v>
       </c>
-      <c r="C59"/>
       <c r="E59" t="s">
-        <v>202</v>
-      </c>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="I59" s="7"/>
-      <c r="J59" s="8"/>
-    </row>
-    <row r="60" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I60" s="7"/>
-      <c r="J60" s="8"/>
+        <v>200</v>
+      </c>
+      <c r="H59" t="s">
+        <v>199</v>
+      </c>
+      <c r="I59" s="4"/>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>130</v>
+      </c>
+      <c r="I60" s="4"/>
+      <c r="J60" s="5"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>55</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>216</v>
+        <v>54</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>214</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E61" t="s">
-        <v>215</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>56</v>
+        <v>213</v>
+      </c>
+      <c r="H61" t="s">
+        <v>55</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>50</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>203</v>
+        <v>49</v>
+      </c>
+      <c r="H62" t="s">
+        <v>201</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D63" s="5"/>
-      <c r="H63" s="5"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2808,7 +2755,7 @@
       <c r="C64">
         <v>0</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D64">
         <f t="shared" ref="D64" si="1">$C$1*C64</f>
         <v>0</v>
       </c>
@@ -2819,7 +2766,7 @@
         <v>40</v>
       </c>
       <c r="H64" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
@@ -2856,138 +2803,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="9"/>
       <c r="C1">
         <f>Main!C1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
       <c r="E4"/>
-      <c r="F4" s="5"/>
+      <c r="F4"/>
       <c r="G4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <f>$C$1*C5</f>
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="F5"/>
       <c r="G5"/>
-      <c r="H5" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="H5" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6"/>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>134</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+        <v>132</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" t="s">
+        <v>211</v>
+      </c>
+      <c r="H7" t="s">
         <v>212</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>214</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <f>$C$1*C8</f>
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>139</v>
+      </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <f>$C$1*C9</f>
         <v>3</v>
       </c>
@@ -3005,15 +2948,15 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>116</v>
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>114</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10">
         <f>$C$1*C10</f>
         <v>3</v>
       </c>
@@ -3021,7 +2964,7 @@
         <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
         <v>27</v>
@@ -3031,13 +2974,12 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>218</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>216</v>
+      </c>
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11">
         <f>$C$1*C11</f>
         <v>6</v>
       </c>
@@ -3045,28 +2987,28 @@
         <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G11" t="s">
         <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>217</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>115</v>
+        <v>215</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12">
         <f t="shared" ref="D12" si="0">$C$1*C12</f>
         <v>6</v>
       </c>
@@ -3083,278 +3025,184 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13">
         <f t="shared" ref="D13" si="1">$C$1*C13</f>
         <v>3</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5" t="s">
-        <v>112</v>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" t="s">
+        <v>110</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="D14" s="5"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="D15" s="5"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="5"/>
-    </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="5"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="5"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D25" s="5"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D26" s="5"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D27" s="5"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D28" s="5"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="D29" s="5"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
-      <c r="D30" s="5"/>
+      <c r="B30" s="6"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="D31" s="5"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="D32" s="5"/>
-      <c r="F32" s="3"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="D33" s="5"/>
-      <c r="F33" s="3"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="D34" s="5"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="D35" s="5"/>
-      <c r="F35" s="3"/>
-      <c r="H35" s="5"/>
+      <c r="F35" s="2"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="D36" s="5"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="5"/>
+      <c r="F36" s="2"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D37" s="5"/>
-      <c r="H37" s="5"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="F38" s="2"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="2"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D41" s="5"/>
-      <c r="H41" s="5"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F42" s="6"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F43" s="6"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="8"/>
-    </row>
-    <row r="44" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F44" s="6"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="8"/>
-    </row>
-    <row r="45" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45"/>
-      <c r="F45" s="6"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46"/>
-      <c r="F46" s="6"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="8"/>
-    </row>
-    <row r="47" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H47" s="10"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H48" s="10"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H49" s="10"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="8"/>
-    </row>
-    <row r="50" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="9"/>
-      <c r="F50" s="6"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="8"/>
-    </row>
-    <row r="51" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
-      <c r="F51" s="6"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="8"/>
-    </row>
-    <row r="52" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="9"/>
-      <c r="F52" s="6"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="8"/>
-    </row>
-    <row r="53" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="E53"/>
-      <c r="F53"/>
-      <c r="G53"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="8"/>
-    </row>
-    <row r="54" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="E54"/>
-      <c r="F54"/>
-      <c r="G54"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="8"/>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F42" s="2"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F43" s="2"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F44" s="2"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="2"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="2"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I47" s="4"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I48" s="4"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="4"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="6"/>
+      <c r="F50" s="2"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="6"/>
+      <c r="F51" s="2"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="6"/>
+      <c r="F52" s="2"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="4"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="4"/>
+      <c r="J54" s="5"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="11"/>
-      <c r="D55" s="5"/>
-      <c r="H55" s="5"/>
+      <c r="B55" s="7"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="13"/>
-      <c r="D56" s="5"/>
-      <c r="H56" s="5"/>
+      <c r="B56" s="8"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
@@ -3362,12 +3210,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D58" s="5"/>
-      <c r="H58" s="5"/>
-    </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D59" s="5"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
@@ -3403,93 +3246,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="9"/>
       <c r="C1">
         <f>Main!C1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>156</v>
+        <v>202</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <f>$C$1*C4</f>
         <v>12</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="10"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>205</v>
+        <v>219</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <f t="shared" ref="D5" si="0">$C$1*C5</f>
         <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>206</v>
+      <c r="F5" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
@@ -3498,56 +3340,52 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="D6" s="5"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="2"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D7" s="5"/>
+      <c r="A7" s="3" t="s">
+        <v>205</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <f t="shared" ref="D8:D9" si="1">$C$1*C8</f>
         <v>3</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="F8" s="6"/>
+      <c r="E8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="10"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>211</v>
+      <c r="A9" t="s">
+        <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -3560,275 +3398,187 @@
       <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="10"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="D10" s="5"/>
+      <c r="A10" t="s">
+        <v>224</v>
+      </c>
       <c r="E10" t="s">
+        <v>220</v>
+      </c>
+      <c r="H10" t="s">
         <v>222</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="5"/>
-    </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D12" s="5"/>
+      <c r="A12" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="D13" s="5"/>
+        <v>224</v>
+      </c>
       <c r="E13" t="s">
-        <v>222</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>220</v>
+      </c>
+      <c r="F13" s="2"/>
       <c r="H13" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D17" s="5"/>
+        <v>221</v>
+      </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D18" s="5"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D19" s="5"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="5"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="5"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="5"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="5"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="D24" s="5"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="D26" s="5"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="D27" s="5"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="D28" s="5"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="D29" s="5"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="D30" s="5"/>
-      <c r="F30" s="3"/>
-      <c r="H30" s="5"/>
+      <c r="F30" s="2"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="D31" s="5"/>
-      <c r="F31" s="3"/>
-      <c r="H31" s="5"/>
+      <c r="F31" s="2"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D32" s="5"/>
-      <c r="H32" s="5"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="F33" s="2"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="5"/>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D36" s="5"/>
-      <c r="H36" s="5"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F37" s="6"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F38" s="6"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="8"/>
-    </row>
-    <row r="39" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F39" s="6"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40"/>
-      <c r="F40" s="6"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41"/>
-      <c r="F41" s="6"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H42" s="10"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H43" s="10"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="8"/>
-    </row>
-    <row r="44" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H44" s="10"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="8"/>
-    </row>
-    <row r="45" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
-      <c r="F45" s="6"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="F46" s="6"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="8"/>
-    </row>
-    <row r="47" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="9"/>
-      <c r="F47" s="6"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="E48"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-      <c r="G49"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="8"/>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F37" s="2"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F38" s="2"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F39" s="2"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F40" s="2"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F41" s="2"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="4"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I43" s="4"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I44" s="4"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="6"/>
+      <c r="F45" s="2"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="6"/>
+      <c r="F46" s="2"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="6"/>
+      <c r="F47" s="2"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I48" s="4"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="4"/>
+      <c r="J49" s="5"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="11"/>
-      <c r="D50" s="5"/>
-      <c r="H50" s="5"/>
+      <c r="B50" s="7"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="13"/>
-      <c r="D51" s="5"/>
-      <c r="H51" s="5"/>
+      <c r="B51" s="8"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
@@ -3836,12 +3586,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D53" s="5"/>
-      <c r="H53" s="5"/>
-    </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D54" s="5"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
@@ -3864,9 +3609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395CB06B-4E35-4D83-939D-902BBC6C7ADF}">
   <dimension ref="A2:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3875,105 +3618,105 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>162</v>
+      <c r="A2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>162</v>
+      <c r="A11" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>162</v>
+      <c r="A18" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>224</v>
+      </c>
+      <c r="B20" t="s">
         <v>226</v>
-      </c>
-      <c r="B20" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B21" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust BOM a tiny bit
</commit_message>
<xml_diff>
--- a/doc/n64adv2_BOM.xlsx
+++ b/doc/n64adv2_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\GitHub\n64rgb_project\n64adv2_pcb\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AB7941-ECB3-4E2D-91F1-2FA04CE7A26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1660AA05-B700-48F7-828C-BC6F0292669A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="198">
   <si>
     <t>Designator</t>
   </si>
@@ -266,12 +266,6 @@
     <t>U6</t>
   </si>
   <si>
-    <t>Buffer gate</t>
-  </si>
-  <si>
-    <t>Alternative: 74LVC1G34DBV</t>
-  </si>
-  <si>
     <t>Clock generator</t>
   </si>
   <si>
@@ -380,12 +374,6 @@
     <t>Aliexpress</t>
   </si>
   <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>74LVC2G17DBV</t>
-  </si>
-  <si>
     <t>TLV70025DDCR</t>
   </si>
   <si>
@@ -552,9 +540,6 @@
   </si>
   <si>
     <t>RN1,RN2,RN3,RN4</t>
-  </si>
-  <si>
-    <t>RC0603FR-0747RL</t>
   </si>
   <si>
     <t>Schmitt-Trigger Buffer</t>
@@ -1484,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1485,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1">
@@ -1544,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1561,7 +1546,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -1569,7 +1554,7 @@
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -1581,7 +1566,7 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -1597,7 +1582,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D56" si="0">$C$1*C6</f>
+        <f t="shared" ref="D6:D55" si="0">$C$1*C6</f>
         <v>3</v>
       </c>
       <c r="E6" t="s">
@@ -1610,7 +1595,7 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1646,7 +1631,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1656,10 +1641,10 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1669,7 +1654,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1695,7 +1680,7 @@
         <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1717,32 +1702,29 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C11">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="E12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" t="s">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
@@ -1751,7 +1733,7 @@
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1761,59 +1743,57 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
       </c>
+      <c r="H13" t="s">
+        <v>112</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>82</v>
-      </c>
       <c r="B14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14">
+        <v>79</v>
+      </c>
+      <c r="E14" t="s">
+        <v>158</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15">
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E14" t="s">
-        <v>161</v>
-      </c>
-      <c r="G14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" t="s">
-        <v>116</v>
-      </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>81</v>
-      </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1823,479 +1803,482 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18">
         <v>1</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B19" t="s">
-        <v>187</v>
-      </c>
-      <c r="C19">
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25">
+        <v>48</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28">
         <v>1</v>
       </c>
-      <c r="D19">
+      <c r="D28">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>84</v>
       </c>
-      <c r="G19" t="s">
+      <c r="B29" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>199</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21">
-        <v>13</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>152</v>
-      </c>
-      <c r="C23">
+      <c r="B30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="D30">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" t="s">
-        <v>154</v>
-      </c>
-      <c r="C24">
-        <v>9</v>
-      </c>
-      <c r="D24">
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
         <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" t="s">
         <v>27</v>
       </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25">
-        <v>8</v>
-      </c>
-      <c r="D25">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" t="s">
         <v>27</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>200</v>
-      </c>
-      <c r="B26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C26">
-        <v>48</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>144</v>
-      </c>
-      <c r="E26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33">
         <v>2</v>
       </c>
-      <c r="D27">
+      <c r="D33">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" t="s">
         <v>27</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34">
         <v>1</v>
       </c>
-      <c r="D29">
+      <c r="D34">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E34" t="s">
         <v>31</v>
       </c>
-      <c r="F29" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="F34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G34" t="s">
         <v>27</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" t="s">
-        <v>27</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" t="s">
         <v>87</v>
       </c>
-      <c r="B31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31">
+      <c r="C37">
         <v>2</v>
       </c>
-      <c r="D31">
+      <c r="D37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G31" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>201</v>
-      </c>
-      <c r="B32" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32">
-        <v>5</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
+      <c r="E37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" t="s">
         <v>15</v>
       </c>
-      <c r="E32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" t="s">
-        <v>27</v>
-      </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="D38">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G33" t="s">
-        <v>27</v>
-      </c>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>163</v>
-      </c>
-      <c r="B34" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G34" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35">
+      <c r="E38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40">
         <v>1</v>
       </c>
-      <c r="D35">
+      <c r="D40">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E35" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="E40" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" t="s">
-        <v>188</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E38" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>138</v>
-      </c>
-      <c r="B39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E39" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" t="s">
-        <v>93</v>
-      </c>
-      <c r="G39" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="5"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2305,21 +2288,21 @@
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2329,7 +2312,7 @@
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" t="s">
@@ -2339,21 +2322,11 @@
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>95</v>
-      </c>
       <c r="B43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" t="s">
@@ -2363,32 +2336,32 @@
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>57</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>164</v>
+        <v>62</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="5"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>55</v>
-      </c>
       <c r="B45" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="E45" t="s">
         <v>62</v>
@@ -2397,195 +2370,181 @@
       <c r="G45" t="s">
         <v>58</v>
       </c>
+      <c r="H45" t="s">
+        <v>67</v>
+      </c>
       <c r="I45" s="4"/>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" t="s">
-        <v>58</v>
-      </c>
-      <c r="H46" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="5"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47">
+      <c r="I47" s="4"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>99</v>
+      </c>
+      <c r="G48" t="s">
+        <v>100</v>
+      </c>
+      <c r="I48" s="4"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="4"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50">
         <v>1</v>
       </c>
-      <c r="D47">
+      <c r="D50">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E47" t="s">
-        <v>133</v>
-      </c>
-      <c r="F47" s="2"/>
-      <c r="G47" t="s">
-        <v>132</v>
-      </c>
-      <c r="I47" s="4"/>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I48" s="4"/>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" t="s">
-        <v>134</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E49" t="s">
-        <v>101</v>
-      </c>
-      <c r="G49" t="s">
-        <v>102</v>
-      </c>
-      <c r="I49" s="4"/>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>154</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="H50" t="s">
+        <v>155</v>
+      </c>
       <c r="I50" s="4"/>
       <c r="J50" s="5"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51" t="s">
-        <v>157</v>
-      </c>
-      <c r="C51">
+      <c r="F51" s="2"/>
+      <c r="H51" t="s">
+        <v>115</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52">
         <v>1</v>
       </c>
-      <c r="D51">
+      <c r="D52">
+        <f>$C$1*C52</f>
+        <v>3</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="H52" t="s">
+        <v>162</v>
+      </c>
+      <c r="I52" s="4"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" t="s">
+        <v>164</v>
+      </c>
+      <c r="H53" t="s">
+        <v>163</v>
+      </c>
+      <c r="I53" s="4"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>116</v>
+      </c>
+      <c r="I54" s="4"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E51" t="s">
-        <v>158</v>
-      </c>
-      <c r="F51" s="2"/>
-      <c r="H51" t="s">
-        <v>159</v>
-      </c>
-      <c r="I51" s="4"/>
-      <c r="J51" s="5"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F52" s="2"/>
-      <c r="H52" t="s">
-        <v>119</v>
-      </c>
-      <c r="I52" s="4"/>
-      <c r="J52" s="5"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>49</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <f>$C$1*C53</f>
-        <v>3</v>
-      </c>
-      <c r="F53" s="2"/>
-      <c r="H53" t="s">
-        <v>166</v>
-      </c>
-      <c r="I53" s="4"/>
-      <c r="J53" s="5"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>35</v>
-      </c>
-      <c r="E54" t="s">
-        <v>168</v>
-      </c>
-      <c r="H54" t="s">
-        <v>167</v>
-      </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>173</v>
+      </c>
       <c r="H55" t="s">
-        <v>120</v>
-      </c>
-      <c r="I55" s="4"/>
-      <c r="J55" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E56" t="s">
-        <v>178</v>
+        <v>45</v>
+      </c>
+      <c r="B56" t="s">
+        <v>197</v>
       </c>
       <c r="H56" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>45</v>
-      </c>
-      <c r="B57" t="s">
-        <v>202</v>
-      </c>
-      <c r="H57" t="s">
-        <v>169</v>
-      </c>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2601,7 +2560,7 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,7 +2573,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1">
@@ -2671,7 +2630,7 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2681,12 +2640,12 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -2695,30 +2654,30 @@
       <c r="A6"/>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H7" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2728,14 +2687,14 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2758,10 +2717,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2784,10 +2743,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2810,7 +2769,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2823,23 +2782,23 @@
         <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2849,10 +2808,10 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -3044,7 +3003,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,7 +3016,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1">
@@ -3102,7 +3061,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3112,7 +3071,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
@@ -3130,10 +3089,10 @@
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3163,10 +3122,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3179,7 +3138,7 @@
         <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -3189,10 +3148,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -3205,7 +3164,7 @@
         <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
@@ -3406,71 +3365,71 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>